<commit_message>
updates to formula and algorithm implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/com/itpaths/rules/price.xlsx
+++ b/src/main/resources/com/itpaths/rules/price.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umesh\Documents\price-poc\src\main\resources\com\itpaths\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0F9151-559A-4181-9DF9-9B2BC89F8B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9B36B8-0C02-4630-AB36-14A8569B7832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>RuleSet</t>
   </si>
@@ -51,15 +51,6 @@
     <t>o.tkt_type_id.equals("$param")</t>
   </si>
   <si>
-    <t>o.diabolo_amt_single==$param</t>
-  </si>
-  <si>
-    <t>o.diabolo_amt_total==$param</t>
-  </si>
-  <si>
-    <t>o.price_natr_id.equals("$param")</t>
-  </si>
-  <si>
     <t>o.setStatus("$param")</t>
   </si>
   <si>
@@ -73,6 +64,69 @@
   </si>
   <si>
     <t>o:PriceRequest</t>
+  </si>
+  <si>
+    <t>price_natr_id.equals("$param")</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_CLASSIC</t>
+  </si>
+  <si>
+    <t>o.setMethod("$param");</t>
+  </si>
+  <si>
+    <t>do_classic</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_CLASSIC_MAX</t>
+  </si>
+  <si>
+    <t>do_classic_max</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_CLASSIC_PLUS</t>
+  </si>
+  <si>
+    <t>do_classic_plus</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_FIXED</t>
+  </si>
+  <si>
+    <t>do_fixed</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_FIXED_PLUS</t>
+  </si>
+  <si>
+    <t>do_fixed_plus</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_ZONE</t>
+  </si>
+  <si>
+    <t>do_zone</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_ZONE_PLUS</t>
+  </si>
+  <si>
+    <t>do_zone_plus</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_MTARIFF</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_MTARIFF_PLUS</t>
+  </si>
+  <si>
+    <t>do_mtariff_plus</t>
+  </si>
+  <si>
+    <t>RTP_T_PN_MTARIFF_MAX</t>
+  </si>
+  <si>
+    <t>SAS_PRICE_ERR</t>
   </si>
 </sst>
 </file>
@@ -88,9 +142,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -155,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,80 +233,59 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,162 +625,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>